<commit_message>
added data and updated spreadsheet
</commit_message>
<xml_diff>
--- a/Project Timeline.xlsx
+++ b/Project Timeline.xlsx
@@ -141,9 +141,6 @@
     <t>M1 Implementation &amp; Coding</t>
   </si>
   <si>
-    <t>Minjae Lee</t>
-  </si>
-  <si>
     <t>M1 Results Evaluation</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>M2 Data Cleaning</t>
+  </si>
+  <si>
+    <t>Minjae Lee</t>
   </si>
   <si>
     <t>M2 Data Visualization</t>
@@ -3347,7 +3347,7 @@
         <v>40</v>
       </c>
       <c r="C22" s="66" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D22" s="44">
         <v>44625.0</v>
@@ -3450,7 +3450,7 @@
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C23" s="66" t="s">
         <v>31</v>
@@ -3556,7 +3556,7 @@
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" s="66" t="s">
         <v>20</v>
@@ -3662,10 +3662,10 @@
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="66" t="s">
         <v>44</v>
-      </c>
-      <c r="C25" s="66" t="s">
-        <v>41</v>
       </c>
       <c r="D25" s="44">
         <v>44627.0</v>
@@ -3983,7 +3983,7 @@
         <v>47</v>
       </c>
       <c r="C28" s="66" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="D28" s="44">
         <v>44633.0</v>
@@ -4820,7 +4820,7 @@
         <v>54</v>
       </c>
       <c r="C36" s="66" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D36" s="45">
         <v>44657.0</v>
@@ -25354,17 +25354,18 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="G6:M6"/>
     <mergeCell ref="M1:T1"/>
+    <mergeCell ref="C3:F3"/>
     <mergeCell ref="G5:AA5"/>
+    <mergeCell ref="AI5:BQ5"/>
     <mergeCell ref="BR5:CS5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="AI5:BQ5"/>
-    <mergeCell ref="AB6:AE6"/>
-    <mergeCell ref="C3:F3"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="N6:T6"/>
     <mergeCell ref="U6:AA6"/>
+    <mergeCell ref="AB6:AE6"/>
+    <mergeCell ref="AI6:AO6"/>
     <mergeCell ref="AP6:AV6"/>
     <mergeCell ref="AW6:BC6"/>
     <mergeCell ref="BD6:BJ6"/>
@@ -25374,7 +25375,6 @@
     <mergeCell ref="BY6:CE6"/>
     <mergeCell ref="CF6:CL6"/>
     <mergeCell ref="CM6:CS6"/>
-    <mergeCell ref="AI6:AO6"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>